<commit_message>
editted excel files - added more pivot tables
</commit_message>
<xml_diff>
--- a/workbooks/daily_activity.xlsx
+++ b/workbooks/daily_activity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\Google data analytics\course 8\week 2\case study 2\Fitabase Data 4.12.16-5.12.16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GDAC-Capstone-Project\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783C0222-BB5D-45B3-9E6E-9DFEDED755DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CA6876-D1F0-4115-AFBF-1DA2FBE6D420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>distance_check</t>
-  </si>
   <si>
     <t>id</t>
   </si>
@@ -83,7 +80,10 @@
     <t>calories</t>
   </si>
   <si>
-    <t>distance_check_less</t>
+    <t>distance_check_greater_total</t>
+  </si>
+  <si>
+    <t>distance_check_less_total_distance</t>
   </si>
 </sst>
 </file>
@@ -644,10 +644,10 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="total_steps"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="total_distance"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="tracker_distance"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="distance_check_less" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="distance_check_less_total_distance" dataDxfId="0">
       <calculatedColumnFormula>IF(D2&lt;E2, "not equal", "equal")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="distance_check">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="distance_check_greater_total">
       <calculatedColumnFormula>IF(D2&gt;E2, "not equal", "equal")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="logged_activities_distance"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:Q941"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F691" sqref="F691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,9 +974,10 @@
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" customWidth="1"/>
-    <col min="8" max="8" width="24.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" customWidth="1"/>
     <col min="9" max="9" width="19.7265625" customWidth="1"/>
     <col min="10" max="10" width="25.90625" customWidth="1"/>
     <col min="11" max="11" width="20.54296875" customWidth="1"/>
@@ -990,55 +991,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>